<commit_message>
identifying & start of enrollment data from ipdes
</commit_message>
<xml_diff>
--- a/data/original/cbtrends-pricing2015.xlsx
+++ b/data/original/cbtrends-pricing2015.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="100" yWindow="100" windowWidth="15620" windowHeight="9060" tabRatio="926"/>
+    <workbookView xWindow="100" yWindow="100" windowWidth="45680" windowHeight="25660" tabRatio="926"/>
   </bookViews>
   <sheets>
     <sheet name="2015 Figures and Tables" sheetId="47" r:id="rId1"/>
@@ -3009,21 +3009,21 @@
   <numFmts count="15">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
-    <numFmt numFmtId="170" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="171" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="172" formatCode="&quot;$&quot;#,##0"/>
-    <numFmt numFmtId="173" formatCode="0.0%"/>
-    <numFmt numFmtId="174" formatCode="&quot;$&quot;#,##0.0"/>
-    <numFmt numFmtId="175" formatCode="#,##0.0"/>
-    <numFmt numFmtId="176" formatCode="&quot;$&quot;#,##0.000"/>
-    <numFmt numFmtId="177" formatCode="&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="178" formatCode="0.0000"/>
-    <numFmt numFmtId="179" formatCode="0.0"/>
-    <numFmt numFmtId="180" formatCode="0.000"/>
-    <numFmt numFmtId="181" formatCode="_([$€-2]* #,##0.00_);_([$€-2]* \(#,##0.00\);_([$€-2]* &quot;-&quot;??_)"/>
-    <numFmt numFmtId="182" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="168" formatCode="&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="169" formatCode="0.0%"/>
+    <numFmt numFmtId="170" formatCode="&quot;$&quot;#,##0.0"/>
+    <numFmt numFmtId="171" formatCode="#,##0.0"/>
+    <numFmt numFmtId="172" formatCode="&quot;$&quot;#,##0.000"/>
+    <numFmt numFmtId="173" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="174" formatCode="0.0000"/>
+    <numFmt numFmtId="175" formatCode="0.0"/>
+    <numFmt numFmtId="176" formatCode="0.000"/>
+    <numFmt numFmtId="177" formatCode="_([$€-2]* #,##0.00_);_([$€-2]* \(#,##0.00\);_([$€-2]* &quot;-&quot;??_)"/>
+    <numFmt numFmtId="178" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="57" x14ac:knownFonts="1">
+  <fonts count="55" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3082,19 +3082,6 @@
     <font>
       <i/>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color indexed="8"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -4078,220 +4065,220 @@
   </borders>
   <cellStyleXfs count="375">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="45" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="46" borderId="24" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="45" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="46" borderId="24" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="181" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="47" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="47" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="39" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="39" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="39" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="39" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="39" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="39" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="39" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="39" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="39" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="39" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="39" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="39" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="39" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="39" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="39" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="39" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="39" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="39" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="39" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="39" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="39" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="39" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="39" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="39" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="39" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="39" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="39" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="39" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="39" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="39" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="39" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="39" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="39" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="39" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="39" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="39" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="39" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="33" fillId="48" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="33" fillId="6" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="49" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="37" fillId="49" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
-    <xf numFmtId="39" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="39" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="39" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="39" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="39" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="39" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="39" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="39" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="39" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="39" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="39" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="39" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="39" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="39" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="39" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="39" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="39" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="39" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="39" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="39" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="39" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="39" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="39" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="39" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="39" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="39" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="39" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="39" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="39" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="39" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="39" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="39" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="39" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="39" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="39" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="39" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="39" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="39" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="48" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="6" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="34" fillId="49" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="35" fillId="49" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
     <xf numFmtId="39" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="39" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
@@ -4301,7 +4288,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
@@ -4329,19 +4316,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
@@ -4354,29 +4341,29 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
@@ -4388,21 +4375,21 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="37" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
@@ -4412,62 +4399,62 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="50" borderId="29" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="50" borderId="29" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="50" borderId="29" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="45" borderId="30" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="6" borderId="30" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="50" borderId="29" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="50" borderId="29" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="45" borderId="30" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="6" borderId="30" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5">
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="31" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="31" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="756">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="39" fillId="51" borderId="0" xfId="337" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="172" fontId="37" fillId="51" borderId="0" xfId="337" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="39" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="37" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -4479,7 +4466,7 @@
     <xf numFmtId="0" fontId="3" fillId="51" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="52" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -4490,10 +4477,10 @@
     <xf numFmtId="3" fontId="2" fillId="51" borderId="7" xfId="347" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="173" fontId="2" fillId="51" borderId="9" xfId="347" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="2" fillId="51" borderId="9" xfId="347" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="173" fontId="2" fillId="51" borderId="10" xfId="347" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="2" fillId="51" borderId="10" xfId="347" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="51" borderId="11" xfId="347" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4502,10 +4489,10 @@
     <xf numFmtId="0" fontId="2" fillId="51" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="172" fontId="2" fillId="51" borderId="0" xfId="347" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="2" fillId="51" borderId="0" xfId="347" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="173" fontId="2" fillId="51" borderId="13" xfId="347" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="2" fillId="51" borderId="13" xfId="347" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="51" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4514,7 +4501,7 @@
     <xf numFmtId="0" fontId="2" fillId="51" borderId="14" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="172" fontId="2" fillId="0" borderId="0" xfId="347" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="347" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="51" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4523,49 +4510,49 @@
     <xf numFmtId="0" fontId="2" fillId="51" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="172" fontId="2" fillId="51" borderId="7" xfId="347" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="2" fillId="51" borderId="7" xfId="347" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="172" fontId="2" fillId="51" borderId="5" xfId="347" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="2" fillId="51" borderId="5" xfId="347" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="172" fontId="2" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="2" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="16" fontId="2" fillId="51" borderId="14" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="172" fontId="2" fillId="51" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="168" fontId="2" fillId="51" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="16" fontId="2" fillId="51" borderId="13" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="172" fontId="2" fillId="51" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="2" fillId="51" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="172" fontId="2" fillId="51" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="2" fillId="51" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="172" fontId="2" fillId="51" borderId="15" xfId="347" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="2" fillId="51" borderId="15" xfId="347" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="173" fontId="2" fillId="51" borderId="0" xfId="347" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="2" fillId="51" borderId="0" xfId="347" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="173" fontId="2" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="2" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="173" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="173" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="52" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4601,7 +4588,7 @@
     <xf numFmtId="16" fontId="2" fillId="51" borderId="16" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="173" fontId="2" fillId="51" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="2" fillId="51" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="51" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4610,10 +4597,10 @@
     <xf numFmtId="0" fontId="2" fillId="51" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="173" fontId="2" fillId="51" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="2" fillId="51" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="2" fillId="51" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -4676,46 +4663,46 @@
     </xf>
     <xf numFmtId="9" fontId="2" fillId="51" borderId="0" xfId="59" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="51" borderId="0" xfId="59" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="172" fontId="2" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="2" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="172" fontId="2" fillId="51" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="2" fillId="51" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="172" fontId="2" fillId="51" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="2" fillId="51" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="52" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="52" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="9" fontId="39" fillId="51" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="37" fillId="51" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="172" fontId="39" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="37" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="172" fontId="39" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="37" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="172" fontId="39" fillId="51" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="37" fillId="51" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="172" fontId="39" fillId="51" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="37" fillId="51" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="172" fontId="39" fillId="51" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="37" fillId="51" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="172" fontId="39" fillId="51" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="37" fillId="51" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="172" fontId="39" fillId="51" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="37" fillId="51" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="9" fontId="39" fillId="51" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="37" fillId="51" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="172" fontId="2" fillId="51" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="2" fillId="51" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="52" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4727,31 +4714,31 @@
     <xf numFmtId="0" fontId="2" fillId="51" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="45" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="43" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="9" fontId="45" fillId="51" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="43" fillId="51" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="3" fontId="45" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="43" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="52" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="51" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="45" fillId="51" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="43" fillId="51" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="51" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="45" fillId="51" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="43" fillId="51" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="9" fontId="45" fillId="51" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="43" fillId="51" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="178" fontId="2" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="178" fontId="1" fillId="52" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="174" fontId="2" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="174" fontId="1" fillId="52" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -4767,19 +4754,19 @@
     <xf numFmtId="0" fontId="2" fillId="51" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="45" fillId="51" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="43" fillId="51" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="45" fillId="51" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="43" fillId="51" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="45" fillId="51" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="43" fillId="51" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="45" fillId="51" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="43" fillId="51" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="4"/>
     </xf>
-    <xf numFmtId="3" fontId="45" fillId="51" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="43" fillId="51" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="4"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="52" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4794,71 +4781,71 @@
     <xf numFmtId="0" fontId="1" fillId="52" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="172" fontId="2" fillId="52" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="2" fillId="52" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="172" fontId="39" fillId="52" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="37" fillId="52" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="172" fontId="39" fillId="52" borderId="11" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="37" fillId="52" borderId="11" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="172" fontId="39" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="172" fontId="39" fillId="51" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="39" fillId="52" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="37" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="168" fontId="37" fillId="51" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="37" fillId="52" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="172" fontId="39" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="37" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="172" fontId="39" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="37" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="2" fillId="51" borderId="17" xfId="59" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="52" borderId="9" xfId="59" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="46" fillId="52" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="44" fillId="52" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="51" borderId="16" xfId="59" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="47" fillId="51" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="45" fillId="51" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="53" borderId="7" xfId="168" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="172" fontId="1" fillId="53" borderId="7" xfId="168" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="1" fillId="53" borderId="7" xfId="168" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="52" borderId="13" xfId="279" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="46" fillId="52" borderId="9" xfId="279" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="2" fillId="52" borderId="7" xfId="279" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="52" borderId="13" xfId="279" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="44" fillId="52" borderId="9" xfId="279" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="2" fillId="52" borderId="7" xfId="279" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="172" fontId="2" fillId="52" borderId="7" xfId="279" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="2" fillId="52" borderId="7" xfId="279" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="172" fontId="39" fillId="52" borderId="7" xfId="279" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="37" fillId="52" borderId="7" xfId="279" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="172" fontId="39" fillId="52" borderId="7" xfId="279" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="37" fillId="52" borderId="7" xfId="279" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="172" fontId="39" fillId="52" borderId="9" xfId="279" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="37" fillId="52" borderId="9" xfId="279" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="39" fillId="52" borderId="9" xfId="279" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="37" fillId="52" borderId="9" xfId="279" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="52" borderId="17" xfId="279" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="52" borderId="17" xfId="279" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="52" borderId="7" xfId="279" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="52" borderId="7" xfId="279" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="52" borderId="7" xfId="279" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4867,14 +4854,14 @@
     <xf numFmtId="0" fontId="2" fillId="52" borderId="7" xfId="279" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="52" borderId="7" xfId="279" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="52" borderId="7" xfId="279" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="39" fillId="52" borderId="8" xfId="279" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="37" fillId="52" borderId="8" xfId="279" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="13" xfId="279" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="2" fillId="51" borderId="0" xfId="168" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="13" xfId="279" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="2" fillId="51" borderId="0" xfId="168" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="9" fontId="2" fillId="51" borderId="13" xfId="168" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4883,37 +4870,37 @@
     <xf numFmtId="9" fontId="2" fillId="51" borderId="14" xfId="168" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="172" fontId="2" fillId="51" borderId="0" xfId="168" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="2" fillId="51" borderId="0" xfId="168" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="172" fontId="2" fillId="51" borderId="13" xfId="168" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="2" fillId="51" borderId="13" xfId="168" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="9" xfId="279" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="2" fillId="51" borderId="15" xfId="168" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="9" xfId="279" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="2" fillId="51" borderId="15" xfId="168" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="172" fontId="2" fillId="51" borderId="7" xfId="168" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="2" fillId="51" borderId="7" xfId="168" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="172" fontId="2" fillId="51" borderId="9" xfId="168" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="2" fillId="51" borderId="9" xfId="168" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="9" fontId="2" fillId="51" borderId="17" xfId="168" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="52" borderId="0" xfId="279" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="46" fillId="52" borderId="10" xfId="279" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="39" fillId="52" borderId="17" xfId="279" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="52" borderId="0" xfId="279" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="44" fillId="52" borderId="10" xfId="279" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="37" fillId="52" borderId="17" xfId="279" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="172" fontId="39" fillId="51" borderId="0" xfId="279" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="37" fillId="51" borderId="0" xfId="279" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="172" fontId="39" fillId="51" borderId="0" xfId="279" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="37" fillId="51" borderId="0" xfId="279" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="172" fontId="39" fillId="51" borderId="7" xfId="279" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="37" fillId="51" borderId="7" xfId="279" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="51" borderId="0" xfId="168" applyFont="1" applyFill="1"/>
@@ -4929,7 +4916,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="168" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="172" fontId="2" fillId="0" borderId="0" xfId="168" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="168" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="168" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -4947,7 +4934,7 @@
     <xf numFmtId="0" fontId="1" fillId="51" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="52" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="52" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="53" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4956,75 +4943,75 @@
     <xf numFmtId="0" fontId="1" fillId="53" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="53" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="39" fillId="53" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="48" fillId="53" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="37" fillId="53" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="37" fillId="53" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="46" fillId="53" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="52" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="52" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="39" fillId="52" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="52" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="37" fillId="52" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="39" fillId="52" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="37" fillId="52" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="39" fillId="52" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="37" fillId="52" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="172" fontId="39" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="172" fontId="39" fillId="51" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="3" fontId="39" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="3" fontId="39" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="168" fontId="37" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="168" fontId="37" fillId="51" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="37" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="37" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="3" fontId="3" fillId="51" borderId="0" xfId="338" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="172" fontId="39" fillId="51" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="37" fillId="51" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="172" fontId="39" fillId="51" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="3" fontId="39" fillId="51" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="168" fontId="37" fillId="51" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="37" fillId="51" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="3" fontId="3" fillId="51" borderId="7" xfId="338" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="172" fontId="39" fillId="51" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="39" fillId="51" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="39" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="39" fillId="51" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="168" fontId="37" fillId="51" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="37" fillId="51" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="37" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="37" fillId="51" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="9" fontId="1" fillId="53" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="52" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="9" fontId="1" fillId="52" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="9" fontId="39" fillId="52" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="37" fillId="52" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="9" fontId="39" fillId="52" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="37" fillId="52" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="9" fontId="39" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="9" fontId="39" fillId="51" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="9" fontId="39" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="39" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="37" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="37" fillId="51" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="37" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="37" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="54" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="54" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="54" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -5034,159 +5021,159 @@
     <xf numFmtId="0" fontId="2" fillId="54" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="168" fontId="0" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="54" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="51" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="0" fillId="51" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="172" fontId="2" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="172" fontId="0" fillId="51" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="51" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="2" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="168" fontId="0" fillId="51" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="46" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="44" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="44" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="39" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="37" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="173" fontId="39" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="37" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="44" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="165" fontId="45" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="43" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="173" fontId="39" fillId="51" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="37" fillId="51" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="165" fontId="39" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="37" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="173" fontId="39" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="37" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="44" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="165" fontId="45" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="43" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="172" fontId="39" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="37" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="39" fillId="51" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="37" fillId="51" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="173" fontId="39" fillId="51" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="37" fillId="51" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="165" fontId="45" fillId="51" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="43" fillId="51" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="52" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="44" fillId="52" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="52" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="52" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="52" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="52" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="52" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="52" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="51" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="51" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="51" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="179" fontId="2" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="175" fontId="2" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="180" fontId="2" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="179" fontId="2" fillId="51" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="175" fontId="2" fillId="51" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="180" fontId="2" fillId="51" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="51" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="52" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="52" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="52" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="52" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="172" fontId="39" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="37" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="172" fontId="39" fillId="51" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="37" fillId="51" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="52" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="52" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="52" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="52" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="51" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5198,385 +5185,385 @@
     <xf numFmtId="0" fontId="2" fillId="51" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="173" fontId="2" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="2" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="52" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="52" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="52" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="52" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="39" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="37" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="173" fontId="39" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="2" fillId="51" borderId="0" xfId="59" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="37" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="2" fillId="51" borderId="0" xfId="59" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="173" fontId="2" fillId="52" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="2" fillId="52" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="52" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="39" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="37" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="9" fontId="39" fillId="51" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="2" fillId="51" borderId="7" xfId="59" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="37" fillId="51" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="2" fillId="51" borderId="7" xfId="59" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="52" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="52" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="39" fillId="52" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="39" fillId="52" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="52" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="37" fillId="52" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="37" fillId="52" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="52" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="52" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="39" fillId="52" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="37" fillId="52" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="172" fontId="39" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="37" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="172" fontId="39" fillId="52" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="37" fillId="52" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="172" fontId="39" fillId="52" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="37" fillId="52" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="172" fontId="39" fillId="51" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="37" fillId="51" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="172" fontId="2" fillId="52" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="2" fillId="52" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="172" fontId="39" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="168" fontId="37" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="52" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="52" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="52" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="52" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="52" borderId="11" xfId="339" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="172" fontId="39" fillId="51" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="37" fillId="51" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="52" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="44" fillId="52" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="172" fontId="39" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="37" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="172" fontId="39" fillId="51" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="37" fillId="51" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="172" fontId="39" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="37" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" indent="1"/>
     </xf>
-    <xf numFmtId="172" fontId="39" fillId="51" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="37" fillId="51" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="52" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="52" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="52" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="52" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="52" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="52" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="52" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="39" fillId="52" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="52" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="37" fillId="52" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="52" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="52" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="52" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="52" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="39" fillId="52" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="37" fillId="52" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="173" fontId="39" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="37" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="4"/>
     </xf>
-    <xf numFmtId="173" fontId="39" fillId="51" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="37" fillId="51" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="4"/>
     </xf>
-    <xf numFmtId="174" fontId="39" fillId="51" borderId="0" xfId="337" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="37" fillId="51" borderId="0" xfId="337" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="175" fontId="39" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="46" fillId="52" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="37" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="44" fillId="52" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="52" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="52" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="39" fillId="51" borderId="7" xfId="337" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="172" fontId="37" fillId="51" borderId="7" xfId="337" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="174" fontId="39" fillId="51" borderId="7" xfId="337" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="37" fillId="51" borderId="7" xfId="337" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="175" fontId="39" fillId="51" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="39" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="177" fontId="39" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="37" fillId="51" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="37" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="173" fontId="37" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="177" fontId="39" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="173" fontId="37" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="19" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="39" fillId="19" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="19" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="173" fontId="37" fillId="19" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="51" borderId="0" xfId="168" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="51" borderId="0" xfId="168" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="39" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="39" fillId="52" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="173" fontId="37" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="37" fillId="52" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="39" fillId="52" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="173" fontId="37" fillId="52" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="51" borderId="7" xfId="168" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="39" fillId="51" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="39" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="173" fontId="37" fillId="51" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="37" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="37" fontId="39" fillId="51" borderId="0" xfId="310" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="39" fillId="51" borderId="0" xfId="357" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="37" fontId="37" fillId="51" borderId="0" xfId="310" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="37" fillId="51" borderId="0" xfId="357" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="52" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="52" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="37" fontId="39" fillId="52" borderId="11" xfId="310" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="37" fontId="37" fillId="52" borderId="11" xfId="310" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="37" fontId="39" fillId="51" borderId="7" xfId="310" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="39" fillId="51" borderId="7" xfId="357" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="37" fontId="37" fillId="51" borderId="7" xfId="310" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="37" fillId="51" borderId="7" xfId="357" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="52" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="52" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="39" fillId="51" borderId="0" xfId="345" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="37" fillId="51" borderId="0" xfId="345" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="39" fillId="51" borderId="13" xfId="345" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="37" fillId="51" borderId="13" xfId="345" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="39" fillId="51" borderId="7" xfId="345" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="37" fillId="51" borderId="7" xfId="345" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="39" fillId="51" borderId="9" xfId="345" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="37" fillId="51" borderId="9" xfId="345" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="52" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="52" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="52" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="52" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="0" xfId="277" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="0" xfId="277" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="51" borderId="0" xfId="170" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="39" fillId="52" borderId="11" xfId="277" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="52" borderId="11" xfId="277" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="51" borderId="7" xfId="170" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="39" fillId="51" borderId="0" xfId="277" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="37" fillId="51" borderId="0" xfId="277" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="39" fillId="51" borderId="7" xfId="277" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="37" fillId="51" borderId="7" xfId="277" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="52" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="44" fillId="52" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="37" fontId="39" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="37" fontId="37" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="37" fontId="39" fillId="51" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="37" fontId="37" fillId="51" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="37" fontId="39" fillId="52" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="37" fontId="37" fillId="52" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="52" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="52" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="39" fillId="51" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="37" fillId="51" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="52" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="52" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="39" fillId="51" borderId="13" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="37" fillId="51" borderId="13" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="39" fillId="51" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="37" fillId="51" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="39" fillId="51" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="37" fillId="51" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="50" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="3" fontId="45" fillId="51" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="48" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="43" fillId="51" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="52" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="52" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="52" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="52" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="4" fontId="39" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="37" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="172" fontId="39" fillId="52" borderId="9" xfId="279" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="37" fillId="52" borderId="9" xfId="279" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="172" fontId="2" fillId="51" borderId="14" xfId="168" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="2" fillId="51" borderId="14" xfId="168" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="172" fontId="39" fillId="52" borderId="10" xfId="279" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="37" fillId="52" borderId="10" xfId="279" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="2" fillId="51" borderId="9" xfId="168" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="172" fontId="46" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="46" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="37" fontId="39" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="44" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="173" fontId="44" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="37" fontId="37" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="51" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="39" fillId="52" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="37" fillId="52" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="39" fillId="52" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="37" fillId="52" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="52" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="52" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="39" fillId="52" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="37" fillId="52" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="39" fillId="52" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="37" fillId="52" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="55" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -5584,104 +5571,104 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="55" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="172" fontId="2" fillId="19" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="2" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="39" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="168" fontId="2" fillId="19" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="2" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="37" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="55" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="172" fontId="39" fillId="51" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="39" fillId="52" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="173" fontId="39" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="173" fontId="39" fillId="51" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="37" fillId="51" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="37" fillId="52" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="37" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="169" fontId="37" fillId="51" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="51" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="39" fillId="52" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="52" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="39" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="37" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="39" fillId="51" borderId="0" xfId="336" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="37" fillId="51" borderId="0" xfId="336" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="52" borderId="7" xfId="336" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="37" fillId="52" borderId="7" xfId="336" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="52" borderId="7" xfId="336" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="37" fillId="52" borderId="7" xfId="336" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="39" fillId="52" borderId="7" xfId="336" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="9" fontId="37" fillId="52" borderId="7" xfId="336" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="39" fillId="52" borderId="7" xfId="336" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="9" fontId="37" fillId="52" borderId="7" xfId="336" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="52" borderId="9" xfId="336" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="37" fillId="52" borderId="9" xfId="336" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="39" fillId="51" borderId="13" xfId="336" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="37" fillId="51" borderId="13" xfId="336" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="52" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="52" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="39" fillId="51" borderId="13" xfId="336" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="37" fillId="51" borderId="13" xfId="336" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="39" fillId="51" borderId="9" xfId="336" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="37" fillId="51" borderId="9" xfId="336" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="39" fillId="51" borderId="7" xfId="336" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="37" fillId="51" borderId="7" xfId="336" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="39" fillId="51" borderId="9" xfId="336" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="37" fillId="51" borderId="9" xfId="336" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="39" fillId="51" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="37" fillId="51" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="52" borderId="17" xfId="336" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="37" fillId="52" borderId="17" xfId="336" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="39" fillId="51" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="37" fillId="51" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="39" fillId="51" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="37" fillId="51" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="39" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="39" fillId="51" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="37" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="37" fillId="51" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="52" borderId="7" xfId="275" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="52" borderId="7" xfId="275" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="52" borderId="7" xfId="275" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="52" borderId="7" xfId="275" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="0" xfId="275" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="0" xfId="275" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="39" fillId="51" borderId="0" xfId="275" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="37" fillId="51" borderId="0" xfId="275" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="7" xfId="275" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="7" xfId="275" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="52" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="52" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="52" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="52" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="51" borderId="0" xfId="154" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -5693,38 +5680,38 @@
     <xf numFmtId="0" fontId="2" fillId="51" borderId="7" xfId="154" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="39" fillId="51" borderId="0" xfId="345" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="37" fillId="51" borderId="0" xfId="345" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" indent="2"/>
     </xf>
-    <xf numFmtId="9" fontId="39" fillId="51" borderId="7" xfId="345" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="37" fillId="51" borderId="7" xfId="345" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="52" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="39" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="37" fillId="52" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="37" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="39" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="37" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="52" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="172" fontId="39" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="39" fillId="52" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="172" fontId="39" fillId="51" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="39" fillId="52" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="37" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="37" fillId="52" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="168" fontId="37" fillId="51" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="37" fillId="52" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="52" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="39" fillId="0" borderId="0" xfId="345" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="37" fillId="0" borderId="0" xfId="345" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="39" fillId="0" borderId="7" xfId="345" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="37" fillId="0" borderId="7" xfId="345" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="2" fillId="51" borderId="7" xfId="227" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5742,31 +5729,31 @@
     <xf numFmtId="0" fontId="2" fillId="51" borderId="0" xfId="229" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="172" fontId="14" fillId="0" borderId="0" xfId="195" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="39" fillId="52" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="12" fillId="0" borderId="0" xfId="195" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="37" fillId="52" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="173" fontId="2" fillId="51" borderId="15" xfId="223" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="173" fontId="2" fillId="51" borderId="5" xfId="223" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="173" fontId="2" fillId="51" borderId="20" xfId="223" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="173" fontId="2" fillId="51" borderId="7" xfId="223" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="173" fontId="2" fillId="51" borderId="7" xfId="221" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="2" fillId="51" borderId="15" xfId="223" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="2" fillId="51" borderId="5" xfId="223" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="2" fillId="51" borderId="20" xfId="223" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="2" fillId="51" borderId="7" xfId="223" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="2" fillId="51" borderId="7" xfId="221" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="51" borderId="7" xfId="221" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="173" fontId="2" fillId="51" borderId="0" xfId="223" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="173" fontId="2" fillId="51" borderId="0" xfId="221" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="169" fontId="2" fillId="51" borderId="0" xfId="223" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="169" fontId="2" fillId="51" borderId="0" xfId="221" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="51" borderId="0" xfId="221" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="52" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="172" fontId="2" fillId="52" borderId="11" xfId="148" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="2" fillId="52" borderId="11" xfId="148" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="52" borderId="11" xfId="330" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="46" fillId="52" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="44" fillId="52" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="333"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="40" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="39" fillId="52" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="52" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="52" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5775,22 +5762,22 @@
     <xf numFmtId="0" fontId="2" fillId="52" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="52" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="52" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="173" fontId="2" fillId="51" borderId="0" xfId="203" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="2" fillId="51" borderId="0" xfId="203" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="173" fontId="2" fillId="51" borderId="0" xfId="214" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="2" fillId="51" borderId="0" xfId="214" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="173" fontId="2" fillId="51" borderId="0" xfId="214" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="2" fillId="51" borderId="0" xfId="214" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="173" fontId="2" fillId="51" borderId="15" xfId="203" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="2" fillId="51" borderId="15" xfId="203" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="173" fontId="2" fillId="51" borderId="7" xfId="214" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="2" fillId="51" borderId="7" xfId="214" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="2"/>
     </xf>
     <xf numFmtId="9" fontId="2" fillId="51" borderId="0" xfId="217" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -5798,21 +5785,21 @@
     <xf numFmtId="9" fontId="2" fillId="51" borderId="0" xfId="219" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="173" fontId="2" fillId="51" borderId="0" xfId="219" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="2" fillId="51" borderId="0" xfId="219" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="173" fontId="2" fillId="51" borderId="7" xfId="219" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="2" fillId="51" borderId="7" xfId="219" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="9" fontId="2" fillId="51" borderId="7" xfId="219" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="9" fontId="39" fillId="51" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="37" fillId="51" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="9" fontId="39" fillId="51" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="37" fillId="51" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="51" borderId="0" xfId="59" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5827,186 +5814,186 @@
     <xf numFmtId="164" fontId="2" fillId="51" borderId="14" xfId="59" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="9" fontId="39" fillId="51" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="9" fontId="39" fillId="51" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="3" fontId="39" fillId="51" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="37" fillId="51" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="37" fillId="51" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="37" fillId="51" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="37" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="3" fontId="39" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="37" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="52" borderId="21" xfId="340" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="39" fillId="52" borderId="21" xfId="340" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="52" borderId="21" xfId="340" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="37" fillId="52" borderId="21" xfId="340" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="52" borderId="21" xfId="340" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="52" borderId="21" xfId="340" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="39" fillId="52" borderId="21" xfId="340" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="37" fillId="52" borderId="21" xfId="340" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="3" fontId="39" fillId="51" borderId="0" xfId="51" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="37" fillId="51" borderId="0" xfId="51" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="9" fontId="39" fillId="51" borderId="0" xfId="345" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="37" fillId="51" borderId="0" xfId="345" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="3" fontId="39" fillId="51" borderId="7" xfId="51" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="37" fillId="51" borderId="7" xfId="51" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="9" fontId="39" fillId="51" borderId="7" xfId="345" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="37" fillId="51" borderId="7" xfId="345" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="172" fontId="39" fillId="51" borderId="0" xfId="65" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="39" fillId="51" borderId="7" xfId="65" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="39" fillId="52" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="37" fillId="51" borderId="0" xfId="65" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="37" fillId="51" borderId="7" xfId="65" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="37" fillId="52" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="0" xfId="148" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="0" xfId="148" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="2" fillId="51" borderId="0" xfId="359" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="0" xfId="148" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="0" xfId="148" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="0" xfId="148" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="0" xfId="148" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="7" xfId="148" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="2" fillId="51" borderId="0" xfId="74" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="7" xfId="148" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="2" fillId="51" borderId="0" xfId="74" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="9" fontId="2" fillId="51" borderId="0" xfId="359" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="0" xfId="148" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="0" xfId="148" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="172" fontId="2" fillId="51" borderId="7" xfId="74" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="2" fillId="51" borderId="7" xfId="74" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="39" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="39" fillId="51" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="39" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="37" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="37" fillId="51" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="37" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="39" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="37" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="39" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="37" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="39" fillId="51" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="37" fillId="51" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="39" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="37" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="39" fillId="51" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="9" fontId="39" fillId="51" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="37" fillId="51" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="37" fillId="51" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="56" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="172" fontId="39" fillId="51" borderId="0" xfId="155" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="172" fontId="39" fillId="51" borderId="7" xfId="155" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="39" fillId="51" borderId="18" xfId="155" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="39" fillId="51" borderId="0" xfId="155" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="173" fontId="8" fillId="52" borderId="11" xfId="339" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="56" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="168" fontId="37" fillId="51" borderId="0" xfId="155" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="168" fontId="37" fillId="51" borderId="7" xfId="155" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="37" fillId="51" borderId="18" xfId="155" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="37" fillId="51" borderId="0" xfId="155" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="8" fillId="52" borderId="11" xfId="339" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="172" fontId="8" fillId="52" borderId="11" xfId="339" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="8" fillId="52" borderId="11" xfId="339" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="top" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" indent="1"/>
     </xf>
-    <xf numFmtId="172" fontId="8" fillId="52" borderId="11" xfId="339" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="8" fillId="52" borderId="11" xfId="339" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="18" xfId="155" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="39" fillId="51" borderId="18" xfId="155" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="18" xfId="155" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="37" fillId="51" borderId="18" xfId="155" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="172" fontId="39" fillId="51" borderId="18" xfId="155" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="37" fillId="51" borderId="18" xfId="155" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" indent="1"/>
     </xf>
-    <xf numFmtId="9" fontId="39" fillId="51" borderId="18" xfId="155" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="0" xfId="155" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="39" fillId="51" borderId="0" xfId="155" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="37" fillId="51" borderId="18" xfId="155" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="0" xfId="155" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="37" fillId="51" borderId="0" xfId="155" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="172" fontId="39" fillId="51" borderId="0" xfId="155" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="37" fillId="51" borderId="0" xfId="155" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" indent="1"/>
     </xf>
-    <xf numFmtId="9" fontId="39" fillId="51" borderId="0" xfId="155" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="7" xfId="155" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="39" fillId="51" borderId="7" xfId="155" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="37" fillId="51" borderId="0" xfId="155" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="7" xfId="155" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="37" fillId="51" borderId="7" xfId="155" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="172" fontId="39" fillId="51" borderId="7" xfId="155" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="37" fillId="51" borderId="7" xfId="155" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" indent="1"/>
     </xf>
-    <xf numFmtId="9" fontId="39" fillId="51" borderId="7" xfId="155" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="0" xfId="155" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="37" fillId="51" borderId="7" xfId="155" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="0" xfId="155" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="4"/>
     </xf>
-    <xf numFmtId="172" fontId="39" fillId="51" borderId="0" xfId="155" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="37" fillId="51" borderId="0" xfId="155" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="0" xfId="155" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="0" xfId="155" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="39" fillId="51" borderId="0" xfId="155" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="37" fillId="51" borderId="0" xfId="155" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="7" xfId="155" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="7" xfId="155" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="4"/>
     </xf>
-    <xf numFmtId="172" fontId="39" fillId="51" borderId="7" xfId="155" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="37" fillId="51" borderId="7" xfId="155" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="7" xfId="155" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="7" xfId="155" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="39" fillId="51" borderId="7" xfId="155" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="37" fillId="51" borderId="7" xfId="155" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="18" xfId="155" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="39" fillId="51" borderId="18" xfId="155" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="18" xfId="155" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="37" fillId="51" borderId="18" xfId="155" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" indent="2"/>
     </xf>
-    <xf numFmtId="9" fontId="39" fillId="51" borderId="18" xfId="155" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="37" fillId="51" borderId="18" xfId="155" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" indent="2"/>
     </xf>
-    <xf numFmtId="172" fontId="39" fillId="51" borderId="0" xfId="155" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="37" fillId="51" borderId="0" xfId="155" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" indent="2"/>
     </xf>
-    <xf numFmtId="9" fontId="39" fillId="51" borderId="0" xfId="155" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="37" fillId="51" borderId="0" xfId="155" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" indent="2"/>
     </xf>
-    <xf numFmtId="9" fontId="39" fillId="51" borderId="7" xfId="155" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="37" fillId="51" borderId="7" xfId="155" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" indent="2"/>
     </xf>
-    <xf numFmtId="172" fontId="39" fillId="51" borderId="7" xfId="155" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="37" fillId="51" borderId="7" xfId="155" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="18" xfId="155" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="39" fillId="51" borderId="18" xfId="155" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="18" xfId="155" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="37" fillId="51" borderId="18" xfId="155" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" indent="2"/>
     </xf>
-    <xf numFmtId="9" fontId="39" fillId="51" borderId="18" xfId="155" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="37" fillId="51" borderId="18" xfId="155" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" indent="2"/>
     </xf>
-    <xf numFmtId="172" fontId="2" fillId="51" borderId="0" xfId="155" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="2" fillId="51" borderId="0" xfId="155" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="51" borderId="0" xfId="155" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -6018,121 +6005,121 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="51" borderId="0" xfId="170" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="39" fillId="52" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="52" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="39" fillId="52" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="37" fillId="52" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="51" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="51" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="51" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="51" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="172" fontId="39" fillId="52" borderId="11" xfId="279" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="37" fillId="52" borderId="11" xfId="279" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="52" borderId="11" xfId="279" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="52" borderId="11" xfId="279" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="172" fontId="2" fillId="51" borderId="16" xfId="168" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="2" fillId="51" borderId="16" xfId="168" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="172" fontId="39" fillId="52" borderId="11" xfId="279" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="37" fillId="52" borderId="11" xfId="279" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="52" borderId="11" xfId="279" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="52" borderId="11" xfId="279" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="168" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="168" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="168" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="168" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="172" fontId="39" fillId="52" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="37" fillId="52" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="52" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="39" fillId="57" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="39" fillId="57" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="52" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="37" fillId="57" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="37" fillId="57" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="182" fontId="39" fillId="51" borderId="7" xfId="65" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="37" fillId="51" borderId="7" xfId="65" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="39" fillId="51" borderId="7" xfId="65" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="37" fillId="51" borderId="7" xfId="65" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="3"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="57" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="39" fillId="57" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="57" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="37" fillId="57" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="57" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="57" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="39" fillId="51" borderId="15" xfId="345" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="37" fillId="51" borderId="15" xfId="345" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="39" fillId="51" borderId="7" xfId="345" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="37" fillId="51" borderId="7" xfId="345" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="51" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="51" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="54" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="52" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="56" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="44" fillId="56" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6183,7 +6170,7 @@
     <xf numFmtId="16" fontId="2" fillId="51" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="53" borderId="7" xfId="59" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6210,7 +6197,7 @@
     <xf numFmtId="0" fontId="1" fillId="52" borderId="9" xfId="168" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="55" fillId="53" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="53" fillId="53" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="51" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6219,10 +6206,10 @@
     <xf numFmtId="0" fontId="1" fillId="56" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="1" fillId="52" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="174" fontId="1" fillId="52" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="1" fillId="52" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="174" fontId="1" fillId="52" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="56" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6240,67 +6227,67 @@
     <xf numFmtId="0" fontId="1" fillId="56" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="56" fillId="56" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="54" fillId="56" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="52" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="52" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="52" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="52" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="52" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="52" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="52" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="52" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="56" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="44" fillId="56" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="56" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="56" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="44" fillId="56" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="57" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="57" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="57" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="57" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="57" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="57" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="52" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="52" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="56" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="44" fillId="56" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="39" fillId="51" borderId="19" xfId="336" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="37" fillId="51" borderId="19" xfId="336" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="39" fillId="51" borderId="11" xfId="336" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="37" fillId="51" borderId="11" xfId="336" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="39" fillId="51" borderId="10" xfId="336" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="37" fillId="51" borderId="10" xfId="336" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="39" fillId="51" borderId="7" xfId="345" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="37" fillId="51" borderId="7" xfId="345" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="56" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="44" fillId="56" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="57" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="57" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="57" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="57" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="56" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="44" fillId="56" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="54" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -7034,7 +7021,7 @@
   </sheetPr>
   <dimension ref="A1:Q62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>

</xml_diff>